<commit_message>
updated java files of sql tables
</commit_message>
<xml_diff>
--- a/Summary AssetCollection.xlsx
+++ b/Summary AssetCollection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\DICT\Andrei\Day53\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\DICT\Andrei\Day54\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23540452-218B-4A2E-8899-5C44706824A6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E01F74-C6B6-4C54-B5BE-28EEAC2EFF17}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="137">
   <si>
     <t>2018-01-001@Bernie@Baltazar@23@IT Department@person</t>
   </si>
@@ -350,6 +350,96 @@
   </si>
   <si>
     <t>Service Date</t>
+  </si>
+  <si>
+    <t>Asset collection ++</t>
+  </si>
+  <si>
+    <t>add assets servlet</t>
+  </si>
+  <si>
+    <t>all assets servlet</t>
+  </si>
+  <si>
+    <t>all locations servlet</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>assetcollection</t>
+  </si>
+  <si>
+    <t>assetmanagerdatabase</t>
+  </si>
+  <si>
+    <t>assetwithlocation</t>
+  </si>
+  <si>
+    <t>assignableasset</t>
+  </si>
+  <si>
+    <t>locationcollection</t>
+  </si>
+  <si>
+    <t>personcollection</t>
+  </si>
+  <si>
+    <t>search servlet</t>
+  </si>
+  <si>
+    <t>software license</t>
+  </si>
+  <si>
+    <t>special to string</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>servicewithlocation</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>DryFold</t>
+  </si>
+  <si>
+    <t>WashDryFold</t>
+  </si>
+  <si>
+    <t>WashDry</t>
+  </si>
+  <si>
+    <t>servicewithcustomer</t>
+  </si>
+  <si>
+    <t>rer</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>SpecialToString</t>
+  </si>
+  <si>
+    <t>ServiceCollection</t>
+  </si>
+  <si>
+    <t>LocationCollection</t>
+  </si>
+  <si>
+    <t>CustomerCollection</t>
   </si>
 </sst>
 </file>
@@ -502,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -576,15 +666,20 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,55 +699,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>66286</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>56595</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F692FAF7-44F3-458A-B581-4AC73C670B89}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14668500" y="4000500"/>
-          <a:ext cx="3114286" cy="4438095"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -680,7 +726,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -693,6 +739,687 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>612775</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50104</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>69290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B258A84-E5CE-470E-BBAB-CDC8D19337A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612775" y="7023100"/>
+          <a:ext cx="5561904" cy="4476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>243657</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>103783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0396DDF5-6D27-4640-B90F-E8835B48C805}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11385550" y="11982450"/>
+          <a:ext cx="6526982" cy="7933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>685031</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>11986</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25EEF65C-B445-4FE5-8DE6-B7AE5C254E68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24180800" y="12014200"/>
+          <a:ext cx="6152381" cy="5714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>494524</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>189862</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA4D03E-ABBF-42BC-A64A-7AC98C18BAFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30848300" y="12039600"/>
+          <a:ext cx="6209524" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>485219</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652F0473-2868-43DE-9960-E59AE9FB7002}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14331950" y="2971800"/>
+          <a:ext cx="4431744" cy="600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>80869</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>554838</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713D626A-FD4A-43C0-B8AC-BBF2F5B835C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15914781" y="3905810"/>
+          <a:ext cx="6256204" cy="6428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>437045</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>159164</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>978804</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>178116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6479A89-3522-4FAA-812A-695D95E2A4B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30574145" y="10636664"/>
+          <a:ext cx="3789784" cy="780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>75511</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>65846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>77657</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>27632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A741EB-AC5B-499A-AA5E-7C2A1152FCFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26431186" y="10543346"/>
+          <a:ext cx="3783571" cy="914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>329293</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>403744</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>77459</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F692FAF7-44F3-458A-B581-4AC73C670B89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27427918" y="3830864"/>
+          <a:ext cx="3112926" cy="4438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>869950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>736029</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>180133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E529711C-3257-44F2-BBB6-A863087EF032}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22520275" y="3924300"/>
+          <a:ext cx="4571429" cy="6733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>124153</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C7D68E8-DC29-4732-959C-F9EFBC3A950E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30756225" y="3800475"/>
+          <a:ext cx="14106853" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>354085</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>258056</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>186434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061857BC-F813-4768-BECD-CEDF48E0069B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18642085" y="11922125"/>
+          <a:ext cx="6190471" cy="7123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>855734</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>62679</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A223038B-70A8-47BB-970C-7995151253A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39193859" y="11772900"/>
+          <a:ext cx="6326883" cy="7581900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605102</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101850</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>165193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64BC848D-04D9-4E22-BE86-C8AA4C4A38A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="605102" y="11672455"/>
+          <a:ext cx="6421983" cy="8495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -997,14 +1724,14 @@
       <c r="L1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1493,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19CEA19-03BB-422A-B6B8-A270ABD6E550}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:BA63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,36 +2245,83 @@
     <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" customWidth="1"/>
+    <col min="30" max="30" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
       <c r="S1" s="15"/>
+      <c r="T1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ1" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>61</v>
       </c>
@@ -1603,8 +2377,65 @@
         <v>73</v>
       </c>
       <c r="S2" s="15"/>
+      <c r="AB2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO2" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU2" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV2" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ2" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="BA2" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>20180001</v>
       </c>
@@ -1633,11 +2464,46 @@
       <c r="N3" s="21"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
       <c r="S3" s="15"/>
+      <c r="AB3" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AJ3" s="26">
+        <v>20180001</v>
+      </c>
+      <c r="AK3" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL3" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM3" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN3" s="27">
+        <v>8</v>
+      </c>
+      <c r="AO3" s="21"/>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="27"/>
+      <c r="AR3" s="27"/>
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="27"/>
+      <c r="AW3" s="21"/>
+      <c r="AX3" s="27"/>
+      <c r="AY3" s="27"/>
+      <c r="AZ3" s="28"/>
+      <c r="BA3" s="28"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>20180002</v>
       </c>
@@ -1666,11 +2532,46 @@
       <c r="N4" s="21"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
       <c r="S4" s="15"/>
+      <c r="AB4" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AJ4" s="26">
+        <v>20180002</v>
+      </c>
+      <c r="AK4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL4" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN4" s="27">
+        <v>5</v>
+      </c>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="27"/>
+      <c r="AQ4" s="27"/>
+      <c r="AR4" s="27"/>
+      <c r="AS4" s="27"/>
+      <c r="AT4" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="27"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="27"/>
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="28"/>
+      <c r="BA4" s="28"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>20180003</v>
       </c>
@@ -1699,11 +2600,46 @@
       <c r="N5" s="21"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
       <c r="S5" s="15"/>
+      <c r="AB5" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AJ5" s="26">
+        <v>20180003</v>
+      </c>
+      <c r="AK5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN5" s="27">
+        <v>10</v>
+      </c>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="27"/>
+      <c r="AQ5" s="27"/>
+      <c r="AR5" s="27"/>
+      <c r="AS5" s="27"/>
+      <c r="AT5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="27"/>
+      <c r="AW5" s="21"/>
+      <c r="AX5" s="27"/>
+      <c r="AY5" s="27"/>
+      <c r="AZ5" s="28"/>
+      <c r="BA5" s="28"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>20180004</v>
       </c>
@@ -1732,11 +2668,48 @@
       <c r="N6" s="21"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
       <c r="S6" s="15"/>
+      <c r="AB6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ6" s="26">
+        <v>20180004</v>
+      </c>
+      <c r="AK6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL6" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM6" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN6" s="27">
+        <v>15</v>
+      </c>
+      <c r="AO6" s="21"/>
+      <c r="AP6" s="27"/>
+      <c r="AQ6" s="27"/>
+      <c r="AR6" s="27"/>
+      <c r="AS6" s="27"/>
+      <c r="AT6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="27"/>
+      <c r="AW6" s="21"/>
+      <c r="AX6" s="27"/>
+      <c r="AY6" s="27"/>
+      <c r="AZ6" s="28"/>
+      <c r="BA6" s="28"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>20180005</v>
       </c>
@@ -1765,11 +2738,48 @@
       <c r="N7" s="21"/>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
       <c r="S7" s="15"/>
+      <c r="AB7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ7" s="26">
+        <v>20180005</v>
+      </c>
+      <c r="AK7" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL7" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN7" s="27">
+        <v>7</v>
+      </c>
+      <c r="AO7" s="21"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="27"/>
+      <c r="AS7" s="27"/>
+      <c r="AT7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="27"/>
+      <c r="AW7" s="21"/>
+      <c r="AX7" s="27"/>
+      <c r="AY7" s="27"/>
+      <c r="AZ7" s="28"/>
+      <c r="BA7" s="28"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
         <v>20180006</v>
       </c>
@@ -1798,11 +2808,46 @@
       <c r="N8" s="21"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
       <c r="S8" s="15"/>
+      <c r="AB8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AJ8" s="26">
+        <v>20180006</v>
+      </c>
+      <c r="AK8" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL8" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN8" s="27">
+        <v>6</v>
+      </c>
+      <c r="AO8" s="21"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="27"/>
+      <c r="AT8" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="27"/>
+      <c r="AW8" s="21"/>
+      <c r="AX8" s="27"/>
+      <c r="AY8" s="27"/>
+      <c r="AZ8" s="28"/>
+      <c r="BA8" s="28"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>20180007</v>
       </c>
@@ -1831,11 +2876,48 @@
       <c r="N9" s="21"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
       <c r="S9" s="15"/>
+      <c r="AB9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ9" s="26">
+        <v>20180007</v>
+      </c>
+      <c r="AK9" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL9" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN9" s="27">
+        <v>8</v>
+      </c>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="27"/>
+      <c r="AS9" s="27"/>
+      <c r="AT9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="27"/>
+      <c r="AW9" s="21"/>
+      <c r="AX9" s="27"/>
+      <c r="AY9" s="27"/>
+      <c r="AZ9" s="28"/>
+      <c r="BA9" s="28"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1864,11 +2946,48 @@
       <c r="N10" s="21"/>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
       <c r="S10" s="15"/>
+      <c r="AB10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="27"/>
+      <c r="AL10" s="27"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="25">
+        <v>1940</v>
+      </c>
+      <c r="AP10" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ10" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR10" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS10" s="27">
+        <v>5</v>
+      </c>
+      <c r="AT10" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="27"/>
+      <c r="AW10" s="21"/>
+      <c r="AX10" s="27"/>
+      <c r="AY10" s="27"/>
+      <c r="AZ10" s="28"/>
+      <c r="BA10" s="28"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1897,11 +3016,54 @@
       <c r="N11" s="21"/>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
       <c r="S11" s="15"/>
+      <c r="AB11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="27"/>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="25">
+        <v>1870</v>
+      </c>
+      <c r="AP11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR11" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS11" s="27">
+        <v>4</v>
+      </c>
+      <c r="AT11" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU11" s="20"/>
+      <c r="AV11" s="27"/>
+      <c r="AW11" s="21"/>
+      <c r="AX11" s="27"/>
+      <c r="AY11" s="27"/>
+      <c r="AZ11" s="28"/>
+      <c r="BA11" s="28"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1930,11 +3092,48 @@
       <c r="N12" s="21"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
       <c r="S12" s="15"/>
+      <c r="AB12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="27"/>
+      <c r="AL12" s="27"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="25">
+        <v>1230</v>
+      </c>
+      <c r="AP12" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ12" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR12" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS12" s="27">
+        <v>7</v>
+      </c>
+      <c r="AT12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="27"/>
+      <c r="AW12" s="21"/>
+      <c r="AX12" s="27"/>
+      <c r="AY12" s="27"/>
+      <c r="AZ12" s="28"/>
+      <c r="BA12" s="28"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1963,15 +3162,56 @@
       <c r="P13" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="Q13" s="29" t="s">
+      <c r="Q13" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="R13" s="29" t="s">
+      <c r="R13" s="28" t="s">
         <v>95</v>
       </c>
       <c r="S13" s="15"/>
+      <c r="AB13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ13" s="20"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="21"/>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27"/>
+      <c r="AR13" s="27"/>
+      <c r="AS13" s="27"/>
+      <c r="AT13" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU13" s="26">
+        <v>20180002</v>
+      </c>
+      <c r="AV13" s="27">
+        <v>20180601</v>
+      </c>
+      <c r="AW13" s="25">
+        <v>1940</v>
+      </c>
+      <c r="AX13" s="27">
+        <v>70</v>
+      </c>
+      <c r="AY13" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AZ13" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA13" s="28" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2000,15 +3240,56 @@
       <c r="P14" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q14" s="29" t="s">
+      <c r="Q14" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="R14" s="29" t="s">
+      <c r="R14" s="28" t="s">
         <v>95</v>
       </c>
       <c r="S14" s="15"/>
+      <c r="AB14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="21"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AR14" s="27"/>
+      <c r="AS14" s="27"/>
+      <c r="AT14" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU14" s="26">
+        <v>20180004</v>
+      </c>
+      <c r="AV14" s="27">
+        <v>20180602</v>
+      </c>
+      <c r="AW14" s="25">
+        <v>1230</v>
+      </c>
+      <c r="AX14" s="27">
+        <v>220</v>
+      </c>
+      <c r="AY14" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ14" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA14" s="28" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -2037,15 +3318,56 @@
       <c r="P15" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Q15" s="29" t="s">
+      <c r="Q15" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="R15" s="29" t="s">
+      <c r="R15" s="28" t="s">
         <v>95</v>
       </c>
       <c r="S15" s="15"/>
+      <c r="AB15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="27"/>
+      <c r="AL15" s="27"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
+      <c r="AO15" s="21"/>
+      <c r="AP15" s="27"/>
+      <c r="AQ15" s="27"/>
+      <c r="AR15" s="27"/>
+      <c r="AS15" s="27"/>
+      <c r="AT15" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU15" s="26">
+        <v>20180005</v>
+      </c>
+      <c r="AV15" s="27">
+        <v>20180603</v>
+      </c>
+      <c r="AW15" s="25">
+        <v>1230</v>
+      </c>
+      <c r="AX15" s="27">
+        <v>100</v>
+      </c>
+      <c r="AY15" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ15" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA15" s="28" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -2074,15 +3396,54 @@
       <c r="P16" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="29" t="s">
+      <c r="Q16" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="R16" s="29" t="s">
+      <c r="R16" s="28" t="s">
         <v>105</v>
       </c>
       <c r="S16" s="15"/>
+      <c r="AB16" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="27"/>
+      <c r="AL16" s="27"/>
+      <c r="AM16" s="27"/>
+      <c r="AN16" s="27"/>
+      <c r="AO16" s="21"/>
+      <c r="AP16" s="27"/>
+      <c r="AQ16" s="27"/>
+      <c r="AR16" s="27"/>
+      <c r="AS16" s="27"/>
+      <c r="AT16" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU16" s="26">
+        <v>20180001</v>
+      </c>
+      <c r="AV16" s="27">
+        <v>20180601</v>
+      </c>
+      <c r="AW16" s="25">
+        <v>1940</v>
+      </c>
+      <c r="AX16" s="27">
+        <v>100</v>
+      </c>
+      <c r="AY16" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ16" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA16" s="28" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2111,15 +3472,62 @@
       <c r="P17" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Q17" s="29" t="s">
+      <c r="Q17" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="R17" s="29" t="s">
+      <c r="R17" s="28" t="s">
         <v>105</v>
       </c>
       <c r="S17" s="15"/>
+      <c r="AB17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="27"/>
+      <c r="AL17" s="27"/>
+      <c r="AM17" s="27"/>
+      <c r="AN17" s="27"/>
+      <c r="AO17" s="21"/>
+      <c r="AP17" s="27"/>
+      <c r="AQ17" s="27"/>
+      <c r="AR17" s="27"/>
+      <c r="AS17" s="27"/>
+      <c r="AT17" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU17" s="26">
+        <v>20180003</v>
+      </c>
+      <c r="AV17" s="27">
+        <v>20180602</v>
+      </c>
+      <c r="AW17" s="25">
+        <v>1870</v>
+      </c>
+      <c r="AX17" s="27">
+        <v>100</v>
+      </c>
+      <c r="AY17" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ17" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA17" s="28" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2148,16 +3556,57 @@
       <c r="P18" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q18" s="29" t="s">
+      <c r="Q18" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="R18" s="29" t="s">
+      <c r="R18" s="28" t="s">
         <v>105</v>
       </c>
       <c r="S18" s="18"/>
       <c r="T18" s="19"/>
+      <c r="AB18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ18" s="20"/>
+      <c r="AK18" s="27"/>
+      <c r="AL18" s="27"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="27"/>
+      <c r="AO18" s="21"/>
+      <c r="AP18" s="27"/>
+      <c r="AQ18" s="27"/>
+      <c r="AR18" s="27"/>
+      <c r="AS18" s="27"/>
+      <c r="AT18" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU18" s="26">
+        <v>20180006</v>
+      </c>
+      <c r="AV18" s="27">
+        <v>20180604</v>
+      </c>
+      <c r="AW18" s="25">
+        <v>1940</v>
+      </c>
+      <c r="AX18" s="27">
+        <v>120</v>
+      </c>
+      <c r="AY18" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ18" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA18" s="28" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2186,20 +3635,90 @@
       <c r="P19" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="Q19" s="29" t="s">
+      <c r="Q19" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="R19" s="29" t="s">
+      <c r="R19" s="28" t="s">
         <v>105</v>
       </c>
       <c r="S19" s="18"/>
       <c r="T19" s="19"/>
+      <c r="AB19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ19" s="20"/>
+      <c r="AK19" s="27"/>
+      <c r="AL19" s="27"/>
+      <c r="AM19" s="27"/>
+      <c r="AN19" s="27"/>
+      <c r="AO19" s="21"/>
+      <c r="AP19" s="27"/>
+      <c r="AQ19" s="27"/>
+      <c r="AR19" s="27"/>
+      <c r="AS19" s="27"/>
+      <c r="AT19" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU19" s="26">
+        <v>20180007</v>
+      </c>
+      <c r="AV19" s="17">
+        <v>20180604</v>
+      </c>
+      <c r="AW19" s="25">
+        <v>1230</v>
+      </c>
+      <c r="AX19" s="27">
+        <v>120</v>
+      </c>
+      <c r="AY19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ19" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA19" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AB20" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="13:51" x14ac:dyDescent="0.25">
+      <c r="AY53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="13:51" x14ac:dyDescent="0.25">
+      <c r="M63" s="32" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="AT1:BA1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="K1:R1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated files for superdrylaundryapp
</commit_message>
<xml_diff>
--- a/Summary AssetCollection.xlsx
+++ b/Summary AssetCollection.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\DICT\Andrei\Day54\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\DICT\Andrei\Day52 project making\GIT\Aquino-Andrei-SuperDry-Laundry-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E01F74-C6B6-4C54-B5BE-28EEAC2EFF17}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3CE20A0-89AA-4415-8B49-1B39FCC5C6DB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ServiceMangerDatabase" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$2:$T$19</definedName>
@@ -1377,16 +1378,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>605102</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>51955</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>156869</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>130396</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>101850</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>165193</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>460440</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>53134</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1409,13 +1410,214 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="605102" y="11672455"/>
+          <a:off x="9267251" y="2416396"/>
           <a:ext cx="6421983" cy="8495238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>29986</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>36408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148446B6-5045-42FA-B8C6-D7FE7E96C1EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="616324" y="196103"/>
+          <a:ext cx="11123809" cy="9057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>480901</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>57706</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6A951F-281B-4DD2-94F3-D0F9EB272064}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11620500" y="201706"/>
+          <a:ext cx="7619048" cy="9000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>341715</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>8406</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7FB352B-2CE6-4E32-BF8D-0081A4B95E98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19296530" y="190501"/>
+          <a:ext cx="9485714" cy="8961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>414618</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>320940</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>69436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F29D04-106D-4439-86DE-C16F6E3AC39B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28855147" y="212912"/>
+          <a:ext cx="5352381" cy="4809524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
@@ -2222,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19CEA19-03BB-422A-B6B8-A270ABD6E550}">
   <dimension ref="A1:BA63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3724,4 +3926,19 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4134C7-CC89-456C-A452-D5D6D76DD1A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AW28" sqref="AW28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>